<commit_message>
entities and db relations
</commit_message>
<xml_diff>
--- a/Web-Excel.xlsx
+++ b/Web-Excel.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CRISTIAN\Desktop\excel_web_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CRISTIAN\Desktop\web-excel_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20564B63-6522-4DEF-B2F9-445DE15F74BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E8C8A5-1FE8-4480-AA00-D1AED937AEEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{1A4F2957-F09E-4C80-B2AA-5C7729BE5827}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{1A4F2957-F09E-4C80-B2AA-5C7729BE5827}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="vistas" sheetId="2" r:id="rId2"/>
     <sheet name="modelado" sheetId="3" r:id="rId3"/>
+    <sheet name="relaciones" sheetId="4" r:id="rId4"/>
+    <sheet name="reglas del negocio" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,10 +27,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="128">
   <si>
     <t>Web excel</t>
   </si>
@@ -161,9 +160,6 @@
     <t>user</t>
   </si>
   <si>
-    <t>funtions</t>
-  </si>
-  <si>
     <t>created at</t>
   </si>
   <si>
@@ -206,63 +202,6 @@
     <t>Modelado de Datos</t>
   </si>
   <si>
-    <t>1. Identificar las entidades del sistema.</t>
-  </si>
-  <si>
-    <t>2. Identificar los atributos de las entidades.</t>
-  </si>
-  <si>
-    <t>3. Identificar las llaves primarias y foráneas.</t>
-  </si>
-  <si>
-    <t>4. Asignar una nomenclatura adeacuada a las entidades y sus atributos.</t>
-  </si>
-  <si>
-    <t>5. Identificar las entidades pivote del sistema.</t>
-  </si>
-  <si>
-    <t>6. Identificar los catálogos del sistema.</t>
-  </si>
-  <si>
-    <t>7. Identificar los tipos de relaciones del sistema.</t>
-  </si>
-  <si>
-    <t>8. Crear el Modelo Entidad-Relación del sistema.</t>
-  </si>
-  <si>
-    <t>9. Crear el Modelo Relacional de la base de datos del sistema.</t>
-  </si>
-  <si>
-    <t>10. Identificar los tipos de dato de los atributos de las entidades del sistema.</t>
-  </si>
-  <si>
-    <t>11. Identificar los atributos que puedan ser únicos en el sistema.</t>
-  </si>
-  <si>
-    <r>
-      <t>12. Identificar las reglas de negocio (Operaciones </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF202225"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>CRUD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF202225"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>) del sistema.</t>
-    </r>
-  </si>
-  <si>
     <t>Entity</t>
   </si>
   <si>
@@ -318,6 +257,168 @@
   </si>
   <si>
     <t>VARCHAR(255)</t>
+  </si>
+  <si>
+    <t>functions</t>
+  </si>
+  <si>
+    <t>shortcut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entidad 1 </t>
+  </si>
+  <si>
+    <t>entidad 2</t>
+  </si>
+  <si>
+    <t>relación</t>
+  </si>
+  <si>
+    <t>type user</t>
+  </si>
+  <si>
+    <t>1:M</t>
+  </si>
+  <si>
+    <t>M:M</t>
+  </si>
+  <si>
+    <t>article_img - pivote</t>
+  </si>
+  <si>
+    <t>article_id PK</t>
+  </si>
+  <si>
+    <t>img_id PK</t>
+  </si>
+  <si>
+    <t>article_category - pivote</t>
+  </si>
+  <si>
+    <t>category_id PK</t>
+  </si>
+  <si>
+    <t>article_shortcut - pivote</t>
+  </si>
+  <si>
+    <t>shortcut_id PK</t>
+  </si>
+  <si>
+    <t>article_functions - pivote</t>
+  </si>
+  <si>
+    <t>function_id PK</t>
+  </si>
+  <si>
+    <t>crear article (solo admin,editor)</t>
+  </si>
+  <si>
+    <t>leer un article (viewers)</t>
+  </si>
+  <si>
+    <t>leer articles (viewers)</t>
+  </si>
+  <si>
+    <t>actualizar article (solo admin,editor)</t>
+  </si>
+  <si>
+    <t>eliminar article (solo admin)</t>
+  </si>
+  <si>
+    <t>crear img (solo admin,editor)</t>
+  </si>
+  <si>
+    <t>leer un img (viewers)</t>
+  </si>
+  <si>
+    <t>leer images (viewers)</t>
+  </si>
+  <si>
+    <t>actualizar img (solo admin,editor)</t>
+  </si>
+  <si>
+    <t>eliminar img (solo admin)</t>
+  </si>
+  <si>
+    <t>crear category (solo admin,editor)</t>
+  </si>
+  <si>
+    <t>leer una category (viewers)</t>
+  </si>
+  <si>
+    <t>leer categories (viewers)</t>
+  </si>
+  <si>
+    <t>actualizar category (solo admin,editor)</t>
+  </si>
+  <si>
+    <t>eliminar category (solo admin)</t>
+  </si>
+  <si>
+    <t>crear shortcut (solo admin,editor)</t>
+  </si>
+  <si>
+    <t>leer un shortcut (viewers)</t>
+  </si>
+  <si>
+    <t>leer shortcuts (viewers)</t>
+  </si>
+  <si>
+    <t>actualizar shortcut (solo admin,editor)</t>
+  </si>
+  <si>
+    <t>eliminar shortcut (solo admin)</t>
+  </si>
+  <si>
+    <t>crear function (solo admin,editor)</t>
+  </si>
+  <si>
+    <t>leer una function (viewers)</t>
+  </si>
+  <si>
+    <t>actualizar function (solo admin,editor)</t>
+  </si>
+  <si>
+    <t>leer functions (viewers)</t>
+  </si>
+  <si>
+    <t>eliminar function (solo admin)</t>
+  </si>
+  <si>
+    <t>crear user (viewers,admin,editor)</t>
+  </si>
+  <si>
+    <t>leer un user (own viewer)</t>
+  </si>
+  <si>
+    <t>leer users (solo admin)</t>
+  </si>
+  <si>
+    <t>actualizar user (solo admin,own viewer)</t>
+  </si>
+  <si>
+    <t>eliminar user (solo admin)</t>
+  </si>
+  <si>
+    <t>crear type_user (solo admin,editor)</t>
+  </si>
+  <si>
+    <t>leer un type_user (solo admin,editor)</t>
+  </si>
+  <si>
+    <t>leer types_users (solo admin,editor)</t>
+  </si>
+  <si>
+    <t>actualizar type_user (solo admin,editor)</t>
+  </si>
+  <si>
+    <t>eliminar type_user (solo admin)</t>
+  </si>
+  <si>
+    <t>Reglas</t>
+  </si>
+  <si>
+    <t>Entidades</t>
   </si>
 </sst>
 </file>
@@ -361,11 +462,12 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF202225"/>
-      <name val="Arial"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -382,7 +484,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -574,11 +676,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -598,6 +758,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -625,14 +793,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -640,6 +800,28 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -657,6 +839,461 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1647825</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>971550</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Conector recto 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{537DB7FB-7703-4239-B663-B6617B9D4309}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1885950" y="704850"/>
+          <a:ext cx="2209800" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1733550</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>981075</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Conector recto 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2143525E-5E2E-4CF3-AD81-9170F0F57D6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1971675" y="742950"/>
+          <a:ext cx="2133600" cy="742950"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1057275</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Conector recto 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DC4699C-894D-4073-9527-CFDAF4C78342}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1295400" y="704851"/>
+          <a:ext cx="2895600" cy="1552574"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1066800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Conector recto 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA00CFEC-F5F3-4990-B506-C2276B367FA6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1304925" y="742950"/>
+          <a:ext cx="2847975" cy="2333625"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1828800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1628775</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Conector recto 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D01EF7E3-B316-41E9-A826-A7CD0765F129}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2066925" y="895350"/>
+          <a:ext cx="5715000" cy="3943350"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1743075</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Conector recto 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA4A7CF5-336C-435D-99ED-AE64F2C403FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1981200" y="1666875"/>
+          <a:ext cx="6400800" cy="3952875"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1714500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1647825</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Conector recto 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{453FDBF3-CDDE-4129-94B8-95CD4D9B93BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1952625" y="2447925"/>
+          <a:ext cx="6400800" cy="38100"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1543050</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1571625</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Conector recto 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E281AA9-2448-4D8A-9249-12F573EE1DB8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1781175" y="3248025"/>
+          <a:ext cx="6496050" cy="428625"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>866775</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Conector recto 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D3B967C-49A6-45D6-B813-F5CA48D18959}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5000625" y="5657850"/>
+          <a:ext cx="3371850" cy="771525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -958,13 +1595,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB4E2EA-8FB0-4E7C-976D-D579492006A0}">
   <dimension ref="A2:D9"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -974,7 +1611,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -988,7 +1625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1000,7 +1637,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1010,19 +1647,19 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1037,11 +1674,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BAAB068-DCB6-4818-9051-3A56496EEEEA}">
   <dimension ref="A1:AB24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" customWidth="1"/>
+    <col min="17" max="17" width="2.42578125" customWidth="1"/>
+    <col min="23" max="23" width="2.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -1079,7 +1725,7 @@
       <c r="AA1" s="5"/>
       <c r="AB1" s="6"/>
     </row>
-    <row r="2" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1105,7 +1751,7 @@
       <c r="AA2" s="11"/>
       <c r="AB2" s="12"/>
     </row>
-    <row r="3" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -1131,7 +1777,7 @@
       <c r="AA3" s="8"/>
       <c r="AB3" s="9"/>
     </row>
-    <row r="4" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>13</v>
       </c>
@@ -1171,7 +1817,7 @@
       <c r="AA4" s="8"/>
       <c r="AB4" s="9"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
@@ -1197,21 +1843,21 @@
       <c r="O5" s="8"/>
       <c r="P5" s="9"/>
       <c r="R5" s="7"/>
-      <c r="S5" s="19" t="s">
+      <c r="S5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="T5" s="20"/>
-      <c r="U5" s="21"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="27"/>
       <c r="V5" s="9"/>
       <c r="X5" s="7"/>
-      <c r="Y5" s="19" t="s">
+      <c r="Y5" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="Z5" s="20"/>
-      <c r="AA5" s="21"/>
+      <c r="Z5" s="26"/>
+      <c r="AA5" s="27"/>
       <c r="AB5" s="9"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
@@ -1237,17 +1883,17 @@
       <c r="O6" s="8"/>
       <c r="P6" s="9"/>
       <c r="R6" s="7"/>
-      <c r="S6" s="22"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="24"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="30"/>
       <c r="V6" s="9"/>
       <c r="X6" s="7"/>
-      <c r="Y6" s="22"/>
-      <c r="Z6" s="23"/>
-      <c r="AA6" s="24"/>
+      <c r="Y6" s="28"/>
+      <c r="Z6" s="29"/>
+      <c r="AA6" s="30"/>
       <c r="AB6" s="9"/>
     </row>
-    <row r="7" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>19</v>
       </c>
@@ -1271,17 +1917,17 @@
       <c r="O7" s="8"/>
       <c r="P7" s="9"/>
       <c r="R7" s="7"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="26"/>
-      <c r="U7" s="27"/>
+      <c r="S7" s="31"/>
+      <c r="T7" s="32"/>
+      <c r="U7" s="33"/>
       <c r="V7" s="9"/>
       <c r="X7" s="7"/>
-      <c r="Y7" s="25"/>
-      <c r="Z7" s="26"/>
-      <c r="AA7" s="27"/>
+      <c r="Y7" s="31"/>
+      <c r="Z7" s="32"/>
+      <c r="AA7" s="33"/>
       <c r="AB7" s="9"/>
     </row>
-    <row r="8" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>20</v>
       </c>
@@ -1315,7 +1961,7 @@
       <c r="AA8" s="8"/>
       <c r="AB8" s="9"/>
     </row>
-    <row r="9" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1345,7 +1991,7 @@
       <c r="AA9" s="8"/>
       <c r="AB9" s="9"/>
     </row>
-    <row r="10" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>13</v>
       </c>
@@ -1380,10 +2026,10 @@
       <c r="X10" s="7"/>
       <c r="Y10" s="15"/>
       <c r="Z10" s="16"/>
-      <c r="AA10" s="28"/>
+      <c r="AA10" s="19"/>
       <c r="AB10" s="9"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>17</v>
       </c>
@@ -1417,7 +2063,7 @@
       <c r="AA11" s="8"/>
       <c r="AB11" s="9"/>
     </row>
-    <row r="12" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
@@ -1453,7 +2099,7 @@
       <c r="AA12" s="8"/>
       <c r="AB12" s="9"/>
     </row>
-    <row r="13" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>19</v>
       </c>
@@ -1486,10 +2132,10 @@
       <c r="X13" s="7"/>
       <c r="Y13" s="15"/>
       <c r="Z13" s="16"/>
-      <c r="AA13" s="28"/>
+      <c r="AA13" s="19"/>
       <c r="AB13" s="9"/>
     </row>
-    <row r="14" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>20</v>
       </c>
@@ -1525,7 +2171,7 @@
       <c r="AA14" s="8"/>
       <c r="AB14" s="9"/>
     </row>
-    <row r="15" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -1553,7 +2199,7 @@
       <c r="AA15" s="8"/>
       <c r="AB15" s="9"/>
     </row>
-    <row r="16" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>13</v>
       </c>
@@ -1586,10 +2232,10 @@
       <c r="X16" s="7"/>
       <c r="Y16" s="15"/>
       <c r="Z16" s="16"/>
-      <c r="AA16" s="28"/>
+      <c r="AA16" s="19"/>
       <c r="AB16" s="9"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>17</v>
       </c>
@@ -1627,7 +2273,7 @@
       <c r="AA17" s="8"/>
       <c r="AB17" s="9"/>
     </row>
-    <row r="18" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>18</v>
       </c>
@@ -1665,7 +2311,7 @@
       <c r="AA18" s="8"/>
       <c r="AB18" s="9"/>
     </row>
-    <row r="19" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>19</v>
       </c>
@@ -1696,10 +2342,10 @@
       <c r="X19" s="7"/>
       <c r="Y19" s="15"/>
       <c r="Z19" s="16"/>
-      <c r="AA19" s="28"/>
+      <c r="AA19" s="19"/>
       <c r="AB19" s="9"/>
     </row>
-    <row r="20" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>20</v>
       </c>
@@ -1723,11 +2369,11 @@
       <c r="O20" s="8"/>
       <c r="P20" s="9"/>
       <c r="R20" s="7"/>
-      <c r="S20" s="19" t="s">
+      <c r="S20" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="T20" s="20"/>
-      <c r="U20" s="21"/>
+      <c r="T20" s="26"/>
+      <c r="U20" s="27"/>
       <c r="V20" s="9"/>
       <c r="X20" s="7"/>
       <c r="Y20" s="8"/>
@@ -1735,7 +2381,7 @@
       <c r="AA20" s="8"/>
       <c r="AB20" s="9"/>
     </row>
-    <row r="21" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -1751,19 +2397,19 @@
       <c r="O21" s="8"/>
       <c r="P21" s="9"/>
       <c r="R21" s="7"/>
-      <c r="S21" s="25"/>
-      <c r="T21" s="26"/>
-      <c r="U21" s="27"/>
+      <c r="S21" s="31"/>
+      <c r="T21" s="32"/>
+      <c r="U21" s="33"/>
       <c r="V21" s="9"/>
       <c r="X21" s="7"/>
-      <c r="Y21" s="19" t="s">
+      <c r="Y21" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="Z21" s="20"/>
-      <c r="AA21" s="21"/>
+      <c r="Z21" s="26"/>
+      <c r="AA21" s="27"/>
       <c r="AB21" s="9"/>
     </row>
-    <row r="22" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
@@ -1786,12 +2432,12 @@
       <c r="U22" s="8"/>
       <c r="V22" s="9"/>
       <c r="X22" s="7"/>
-      <c r="Y22" s="25"/>
-      <c r="Z22" s="26"/>
-      <c r="AA22" s="27"/>
+      <c r="Y22" s="31"/>
+      <c r="Z22" s="32"/>
+      <c r="AA22" s="33"/>
       <c r="AB22" s="9"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -1819,7 +2465,7 @@
       <c r="AA23" s="8"/>
       <c r="AB23" s="9"/>
     </row>
-    <row r="24" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -1858,465 +2504,405 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8EF0FF-E96C-4F6D-B408-A36370844E92}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
       <c r="D1" s="36"/>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="13" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="13" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="13" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="14" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="33" t="s">
-        <v>52</v>
+      <c r="B13" s="24" t="s">
+        <v>51</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="13" t="s">
         <v>36</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="13" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="13" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="13" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="14" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="33" t="s">
-        <v>45</v>
+      <c r="B20" s="24" t="s">
+        <v>44</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
       <c r="B22" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="33" t="s">
-        <v>48</v>
+      <c r="B23" s="24" t="s">
+        <v>47</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="13" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="14" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="33" t="s">
-        <v>50</v>
+        <v>74</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>49</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="13" t="s">
         <v>17</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" s="14" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B31" s="33" t="s">
-        <v>71</v>
+        <v>64</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>58</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B33" s="33" t="s">
-        <v>76</v>
+        <v>65</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>63</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A36" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A37" s="29" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A38" s="29" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A39" s="29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A40" s="29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A41" s="29" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A42" s="29" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A43" s="29" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A44" s="29" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A45" s="29" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A46" s="29" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="29" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2325,4 +2911,623 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A83A3C0-1689-4DAF-91F7-39783890D299}">
+  <dimension ref="B2:J34"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="7"/>
+      <c r="E6" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="8"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" s="37"/>
+    </row>
+    <row r="13" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G14" s="7"/>
+      <c r="H14" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="H15" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="40" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G18" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="J18" s="37"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G19" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G20" s="7"/>
+      <c r="H20" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G21" s="10"/>
+      <c r="H21" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="7"/>
+      <c r="E24" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D25" s="7"/>
+      <c r="E25" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="7"/>
+      <c r="E26" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G26" s="10"/>
+      <c r="H26" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="7"/>
+      <c r="E27" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="7"/>
+      <c r="E28" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H28" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="10"/>
+      <c r="E29" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H29" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G30" s="10"/>
+      <c r="H30" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="20"/>
+    </row>
+    <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G32" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H32" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G33" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H33" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="7:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G34" s="10"/>
+      <c r="H34" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7178C9-9D29-4984-A067-6DC1A7082AF5}">
+  <dimension ref="B1:C37"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.5703125" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="47" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="44"/>
+      <c r="C4" s="39" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="44"/>
+      <c r="C5" s="39" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="44"/>
+      <c r="C6" s="39" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="45"/>
+      <c r="C7" s="40" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="44"/>
+      <c r="C9" s="39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="44"/>
+      <c r="C10" s="39" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="44"/>
+      <c r="C11" s="39" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="45"/>
+      <c r="C12" s="40" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="44"/>
+      <c r="C14" s="39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="44"/>
+      <c r="C15" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="44"/>
+      <c r="C16" s="39" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="45"/>
+      <c r="C17" s="40" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="44"/>
+      <c r="C19" s="39" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="44"/>
+      <c r="C20" s="39" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="44"/>
+      <c r="C21" s="39" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="45"/>
+      <c r="C22" s="40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="46" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="44"/>
+      <c r="C24" s="39" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="44"/>
+      <c r="C25" s="39" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="44"/>
+      <c r="C26" s="39" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="45"/>
+      <c r="C27" s="40" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="46" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="44"/>
+      <c r="C29" s="39" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="44"/>
+      <c r="C30" s="39" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="44"/>
+      <c r="C31" s="39" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="45"/>
+      <c r="C32" s="40" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="46" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="44"/>
+      <c r="C34" s="39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="44"/>
+      <c r="C35" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="44"/>
+      <c r="C36" s="39" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="45"/>
+      <c r="C37" s="40" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B33:B37"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="B28:B32"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>